<commit_message>
BE data preperation WW (qg21) and annualSimulation checking and considering of WW generation
</commit_message>
<xml_diff>
--- a/data_preprocessing/breitenerhebung/BE_data/BE_BuildingData_Dummy.xlsx
+++ b/data_preprocessing/breitenerhebung/BE_data/BE_BuildingData_Dummy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\DIBS---Dynamic-ISO-Building-Simulator-master\data_preprocessing\breitenerhebung\BE_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/d17128779_mytudublin_ie/Documents/GitHub/DIBS---Dynamic-ISO-Building-Simulator/data_preprocessing/breitenerhebung/BE_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE12C6E-26C8-471C-968F-7BA59BE8B769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{6AE12C6E-26C8-471C-968F-7BA59BE8B769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09C0923A-5353-45C4-8CFC-FF2DCF0CE1C7}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="110">
   <si>
     <t>scr_gebaeude_id</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>AB123456_1_08</t>
+  </si>
+  <si>
+    <t>qg21</t>
   </si>
 </sst>
 </file>
@@ -739,24 +742,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ10"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AK12" sqref="AK12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -865,8 +868,11 @@
       <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AK1" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -975,8 +981,11 @@
       <c r="AJ2">
         <v>1.55</v>
       </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1085,8 +1094,11 @@
       <c r="AJ3">
         <v>0.71020000000000005</v>
       </c>
+      <c r="AK3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1195,8 +1207,11 @@
       <c r="AJ4">
         <v>2</v>
       </c>
+      <c r="AK4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -1305,8 +1320,11 @@
       <c r="AJ5">
         <v>0.81559999999999999</v>
       </c>
+      <c r="AK5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -1415,8 +1433,11 @@
       <c r="AJ6">
         <v>0.73809999999999998</v>
       </c>
+      <c r="AK6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -1525,8 +1546,11 @@
       <c r="AJ7">
         <v>0.3553</v>
       </c>
+      <c r="AK7">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -1635,8 +1659,11 @@
       <c r="AJ8">
         <v>0.40989999999999999</v>
       </c>
+      <c r="AK8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -1745,8 +1772,11 @@
       <c r="AJ9">
         <v>0.40989999999999999</v>
       </c>
+      <c r="AK9">
+        <v>3</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -1854,6 +1884,9 @@
       </c>
       <c r="AJ10">
         <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>